<commit_message>
fully tested for jack to add to his spreadsheet
</commit_message>
<xml_diff>
--- a/Testing Spreadsheet v1.0 Order Page Meat Extravaganza pizza - Adam Hale.xlsx
+++ b/Testing Spreadsheet v1.0 Order Page Meat Extravaganza pizza - Adam Hale.xlsx
@@ -5,7 +5,7 @@
   <workbookPr autoCompressPictures="0"/>
   <workbookProtection workbookPassword="A6C2" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24840" windowHeight="15600" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="1080" yWindow="120" windowWidth="24840" windowHeight="15600" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Reqs" sheetId="5" r:id="rId1"/>
@@ -200,7 +200,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="200">
   <si>
     <t xml:space="preserve">Req </t>
   </si>
@@ -592,30 +592,6 @@
     <t>Check that the correct price is displayed after the meat extravaganza pizza, with pepporioni, is added to the cart</t>
   </si>
   <si>
-    <t>The total amount is incorrect due to incorrect pizza price</t>
-  </si>
-  <si>
-    <t>The pizza is the wrong price due to incorrect pizza price</t>
-  </si>
-  <si>
-    <t>The onions topping was not added to cart</t>
-  </si>
-  <si>
-    <t>total was incorrect due to incorrect pizza price as well as not adding onions to the cart</t>
-  </si>
-  <si>
-    <t xml:space="preserve">total was incorrect due to incorrect pizza price </t>
-  </si>
-  <si>
-    <t>The total amount is incorrect due to both incorrect pizza price and extra price for peppers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The total amount is incorrect due to both incorrect pizza price and extra price for peppers </t>
-  </si>
-  <si>
-    <t>The total amount is incorrect due to both incorrect pizza price and extra price for peppers as well as the onions topping was not added to cart</t>
-  </si>
-  <si>
     <t>On adding the meat extravaganza pizza to the basket.</t>
   </si>
   <si>
@@ -818,6 +794,48 @@
   </si>
   <si>
     <t>To show that as a user I can add one or more combinations of toppings to the meat extravaganza pizza and each topping/combination will be displayed in the cart along with the correct price.</t>
+  </si>
+  <si>
+    <t>The pizza is the wrong price due to incorrect pizza price. Failed on all borwsers and mobile devices</t>
+  </si>
+  <si>
+    <t>The total amount is incorrect due to incorrect pizza price. Failed on all browsers and mobile devices</t>
+  </si>
+  <si>
+    <t>The total amount is incorrect due to both incorrect pizza price and extra price for peppers. Faied on all browsers and mobile devices</t>
+  </si>
+  <si>
+    <t>The onions topping was not added to cart. Failed on all browsers and mobile devices</t>
+  </si>
+  <si>
+    <t>total was incorrect due to incorrect pizza price as well as not adding onions to the cart. Failed on all browsers and mobile devices</t>
+  </si>
+  <si>
+    <t>total was incorrect due to incorrect pizza price. Failed on all browsers and mobile devices</t>
+  </si>
+  <si>
+    <t>The total amount is incorrect due to both incorrect pizza price and extra price for peppers. Failed on all browsers and mobile devices</t>
+  </si>
+  <si>
+    <t>The total amount is incorrect due to both incorrect pizza price and extra price for peppers. Failed on all browsers and mobile devies</t>
+  </si>
+  <si>
+    <t>The onions topping was not added to cart. Failed on all browsers and all mobile devices</t>
+  </si>
+  <si>
+    <t>The total amount is incorrect due to both incorrect pizza price and extra price for peppers as well as the onions topping was not added to cart.  Failed on all browsers and mobile devices</t>
+  </si>
+  <si>
+    <t>The onions topping was not added to cart.  Failed on all browsers and mobile devices</t>
+  </si>
+  <si>
+    <t>total was incorrect due to incorrect pizza price as well as not adding onions to the cart.  Failed on all browsers and mobile devices</t>
+  </si>
+  <si>
+    <t>The total amount is incorrect due to both incorrect pizza price and extra price for peppers.  Failed on all browsers and mobile devices</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Automated Selenium Test </t>
   </si>
 </sst>
 </file>
@@ -1017,8 +1035,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="401">
+  <cellStyleXfs count="403">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1510,7 +1530,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="401">
+  <cellStyles count="403">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1711,6 +1731,7 @@
     <cellStyle name="Followed Hyperlink" xfId="396" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="398" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="400" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="402" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1911,6 +1932,7 @@
     <cellStyle name="Hyperlink" xfId="395" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="397" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="399" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="401" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="1">
@@ -1971,6 +1993,7 @@
           <c:dLbls>
             <c:dLbl>
               <c:idx val="0"/>
+              <c:layout/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
               <c:showCatName val="0"/>
@@ -1985,6 +2008,7 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="1"/>
+              <c:layout/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
               <c:showCatName val="0"/>
@@ -2070,6 +2094,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2139,7 +2164,7 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.0</c:v>
@@ -2160,11 +2185,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2137422072"/>
-        <c:axId val="2124364872"/>
+        <c:axId val="2115932888"/>
+        <c:axId val="2115935832"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2137422072"/>
+        <c:axId val="2115932888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2174,7 +2199,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2124364872"/>
+        <c:crossAx val="2115935832"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2182,7 +2207,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2124364872"/>
+        <c:axId val="2115935832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2193,7 +2218,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2137422072"/>
+        <c:crossAx val="2115932888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2606,7 +2631,7 @@
   </sheetPr>
   <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -2636,7 +2661,7 @@
         <v>62</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>55</v>
@@ -2653,7 +2678,7 @@
         <v>63</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>55</v>
@@ -2774,8 +2799,8 @@
   </sheetPr>
   <dimension ref="A1:U146"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView topLeftCell="K1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
+      <selection activeCell="L34" sqref="L34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -2850,7 +2875,7 @@
         <v>66</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>58</v>
@@ -2889,7 +2914,7 @@
         <v>67</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>58</v>
@@ -2919,7 +2944,7 @@
         <v>33</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>53</v>
+        <v>35</v>
       </c>
       <c r="M3" s="33">
         <v>42089</v>
@@ -2928,7 +2953,7 @@
         <v>116</v>
       </c>
       <c r="O3" s="9" t="s">
-        <v>119</v>
+        <v>186</v>
       </c>
       <c r="P3" s="10"/>
       <c r="T3" s="27" t="s">
@@ -2940,7 +2965,7 @@
         <v>68</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>58</v>
@@ -2976,7 +3001,7 @@
         <v>69</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>58</v>
@@ -3006,7 +3031,7 @@
         <v>33</v>
       </c>
       <c r="L5" s="4" t="s">
-        <v>53</v>
+        <v>35</v>
       </c>
       <c r="M5" s="33">
         <v>42089</v>
@@ -3015,7 +3040,7 @@
         <v>116</v>
       </c>
       <c r="O5" s="9" t="s">
-        <v>118</v>
+        <v>187</v>
       </c>
       <c r="P5" s="10"/>
     </row>
@@ -3024,7 +3049,7 @@
         <v>70</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>58</v>
@@ -3097,7 +3122,7 @@
         <v>33</v>
       </c>
       <c r="L7" s="4" t="s">
-        <v>53</v>
+        <v>35</v>
       </c>
       <c r="M7" s="33">
         <v>42089</v>
@@ -3106,7 +3131,7 @@
         <v>116</v>
       </c>
       <c r="O7" s="9" t="s">
-        <v>118</v>
+        <v>187</v>
       </c>
       <c r="P7" s="10"/>
       <c r="T7" t="s">
@@ -3122,7 +3147,7 @@
         <v>72</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>58</v>
@@ -3158,7 +3183,7 @@
         <v>73</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>58</v>
@@ -3188,7 +3213,7 @@
         <v>33</v>
       </c>
       <c r="L9" s="4" t="s">
-        <v>53</v>
+        <v>35</v>
       </c>
       <c r="M9" s="33">
         <v>42089</v>
@@ -3197,7 +3222,7 @@
         <v>116</v>
       </c>
       <c r="O9" s="9" t="s">
-        <v>124</v>
+        <v>188</v>
       </c>
       <c r="P9" s="10"/>
     </row>
@@ -3206,7 +3231,7 @@
         <v>74</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>58</v>
@@ -3236,7 +3261,7 @@
         <v>33</v>
       </c>
       <c r="L10" s="4" t="s">
-        <v>53</v>
+        <v>35</v>
       </c>
       <c r="M10" s="33">
         <v>42089</v>
@@ -3245,7 +3270,7 @@
         <v>116</v>
       </c>
       <c r="O10" s="10" t="s">
-        <v>120</v>
+        <v>189</v>
       </c>
       <c r="P10" s="10"/>
     </row>
@@ -3254,7 +3279,7 @@
         <v>60</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>58</v>
@@ -3284,7 +3309,7 @@
         <v>33</v>
       </c>
       <c r="L11" s="4" t="s">
-        <v>53</v>
+        <v>35</v>
       </c>
       <c r="M11" s="33">
         <v>42089</v>
@@ -3293,7 +3318,7 @@
         <v>116</v>
       </c>
       <c r="O11" s="10" t="s">
-        <v>121</v>
+        <v>190</v>
       </c>
       <c r="P11" s="10"/>
     </row>
@@ -3302,7 +3327,7 @@
         <v>75</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>58</v>
@@ -3338,7 +3363,7 @@
         <v>76</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>58</v>
@@ -3368,7 +3393,7 @@
         <v>33</v>
       </c>
       <c r="L13" s="4" t="s">
-        <v>53</v>
+        <v>35</v>
       </c>
       <c r="M13" s="33">
         <v>42089</v>
@@ -3377,7 +3402,7 @@
         <v>116</v>
       </c>
       <c r="O13" s="10" t="s">
-        <v>122</v>
+        <v>191</v>
       </c>
       <c r="P13" s="10"/>
     </row>
@@ -3386,7 +3411,7 @@
         <v>77</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>58</v>
@@ -3422,7 +3447,7 @@
         <v>78</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>58</v>
@@ -3452,7 +3477,7 @@
         <v>33</v>
       </c>
       <c r="L15" s="4" t="s">
-        <v>53</v>
+        <v>35</v>
       </c>
       <c r="M15" s="33">
         <v>42089</v>
@@ -3461,7 +3486,7 @@
         <v>116</v>
       </c>
       <c r="O15" s="9" t="s">
-        <v>123</v>
+        <v>192</v>
       </c>
       <c r="P15" s="10"/>
     </row>
@@ -3470,7 +3495,7 @@
         <v>79</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>58</v>
@@ -3500,7 +3525,7 @@
         <v>33</v>
       </c>
       <c r="L16" s="4" t="s">
-        <v>53</v>
+        <v>35</v>
       </c>
       <c r="M16" s="33">
         <v>42089</v>
@@ -3509,7 +3534,7 @@
         <v>116</v>
       </c>
       <c r="O16" s="10" t="s">
-        <v>120</v>
+        <v>189</v>
       </c>
       <c r="P16" s="10"/>
     </row>
@@ -3518,7 +3543,7 @@
         <v>80</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>58</v>
@@ -3548,7 +3573,7 @@
         <v>33</v>
       </c>
       <c r="L17" s="4" t="s">
-        <v>53</v>
+        <v>35</v>
       </c>
       <c r="M17" s="33">
         <v>42089</v>
@@ -3557,7 +3582,7 @@
         <v>116</v>
       </c>
       <c r="O17" s="10" t="s">
-        <v>121</v>
+        <v>190</v>
       </c>
       <c r="P17" s="10"/>
     </row>
@@ -3566,7 +3591,7 @@
         <v>81</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>58</v>
@@ -3609,7 +3634,7 @@
         <v>82</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>58</v>
@@ -3639,7 +3664,7 @@
         <v>33</v>
       </c>
       <c r="L19" s="4" t="s">
-        <v>53</v>
+        <v>35</v>
       </c>
       <c r="M19" s="33">
         <v>42089</v>
@@ -3648,7 +3673,7 @@
         <v>116</v>
       </c>
       <c r="O19" s="9" t="s">
-        <v>123</v>
+        <v>193</v>
       </c>
       <c r="P19" s="10"/>
       <c r="T19" t="s">
@@ -3656,7 +3681,7 @@
       </c>
       <c r="U19" s="31">
         <f>COUNTIF(L2:L5,"*Moderate*")</f>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:21" ht="52">
@@ -3664,7 +3689,7 @@
         <v>83</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>58</v>
@@ -3694,7 +3719,7 @@
         <v>33</v>
       </c>
       <c r="L20" s="4" t="s">
-        <v>53</v>
+        <v>35</v>
       </c>
       <c r="M20" s="33">
         <v>42089</v>
@@ -3703,7 +3728,7 @@
         <v>116</v>
       </c>
       <c r="O20" s="10" t="s">
-        <v>120</v>
+        <v>194</v>
       </c>
       <c r="P20" s="10"/>
       <c r="T20" t="s">
@@ -3719,7 +3744,7 @@
         <v>84</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>58</v>
@@ -3749,7 +3774,7 @@
         <v>33</v>
       </c>
       <c r="L21" s="4" t="s">
-        <v>53</v>
+        <v>35</v>
       </c>
       <c r="M21" s="32">
         <v>42089</v>
@@ -3758,7 +3783,7 @@
         <v>116</v>
       </c>
       <c r="O21" s="10" t="s">
-        <v>121</v>
+        <v>190</v>
       </c>
       <c r="P21" s="10"/>
       <c r="T21" t="s">
@@ -3774,7 +3799,7 @@
         <v>85</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>58</v>
@@ -3804,7 +3829,7 @@
         <v>33</v>
       </c>
       <c r="L22" s="4" t="s">
-        <v>53</v>
+        <v>35</v>
       </c>
       <c r="M22" s="32">
         <v>42089</v>
@@ -3813,7 +3838,7 @@
         <v>116</v>
       </c>
       <c r="O22" s="10" t="s">
-        <v>120</v>
+        <v>189</v>
       </c>
       <c r="P22" s="10"/>
     </row>
@@ -3822,7 +3847,7 @@
         <v>86</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>58</v>
@@ -3852,7 +3877,7 @@
         <v>33</v>
       </c>
       <c r="L23" s="4" t="s">
-        <v>53</v>
+        <v>35</v>
       </c>
       <c r="M23" s="32">
         <v>42089</v>
@@ -3861,7 +3886,7 @@
         <v>116</v>
       </c>
       <c r="O23" s="9" t="s">
-        <v>125</v>
+        <v>195</v>
       </c>
       <c r="P23" s="10"/>
     </row>
@@ -3870,7 +3895,7 @@
         <v>87</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>58</v>
@@ -3909,7 +3934,7 @@
         <v>116</v>
       </c>
       <c r="O24" s="10" t="s">
-        <v>120</v>
+        <v>196</v>
       </c>
       <c r="P24" s="10"/>
     </row>
@@ -3918,7 +3943,7 @@
         <v>88</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>58</v>
@@ -3957,7 +3982,7 @@
         <v>116</v>
       </c>
       <c r="O25" s="9" t="s">
-        <v>125</v>
+        <v>195</v>
       </c>
       <c r="P25" s="10"/>
     </row>
@@ -3966,7 +3991,7 @@
         <v>89</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>58</v>
@@ -4005,7 +4030,7 @@
         <v>116</v>
       </c>
       <c r="O26" s="10" t="s">
-        <v>120</v>
+        <v>196</v>
       </c>
       <c r="P26" s="10"/>
     </row>
@@ -4014,7 +4039,7 @@
         <v>90</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>58</v>
@@ -4053,7 +4078,7 @@
         <v>116</v>
       </c>
       <c r="O27" s="9" t="s">
-        <v>125</v>
+        <v>195</v>
       </c>
       <c r="P27" s="10"/>
     </row>
@@ -4062,7 +4087,7 @@
         <v>91</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>58</v>
@@ -4101,7 +4126,7 @@
         <v>116</v>
       </c>
       <c r="O28" s="10" t="s">
-        <v>120</v>
+        <v>196</v>
       </c>
       <c r="P28" s="10"/>
     </row>
@@ -4110,7 +4135,7 @@
         <v>92</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>58</v>
@@ -4140,7 +4165,7 @@
         <v>33</v>
       </c>
       <c r="L29" s="4" t="s">
-        <v>53</v>
+        <v>35</v>
       </c>
       <c r="M29" s="32">
         <v>42089</v>
@@ -4149,7 +4174,7 @@
         <v>116</v>
       </c>
       <c r="O29" s="10" t="s">
-        <v>121</v>
+        <v>197</v>
       </c>
       <c r="P29" s="10"/>
     </row>
@@ -4158,7 +4183,7 @@
         <v>93</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>58</v>
@@ -4194,7 +4219,7 @@
         <v>94</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>58</v>
@@ -4224,7 +4249,7 @@
         <v>33</v>
       </c>
       <c r="L31" s="4" t="s">
-        <v>53</v>
+        <v>35</v>
       </c>
       <c r="M31" s="32">
         <v>42089</v>
@@ -4233,7 +4258,7 @@
         <v>116</v>
       </c>
       <c r="O31" s="9" t="s">
-        <v>123</v>
+        <v>198</v>
       </c>
       <c r="P31" s="10"/>
     </row>
@@ -4242,7 +4267,7 @@
         <v>95</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="C32" s="3" t="s">
         <v>58</v>
@@ -4272,7 +4297,7 @@
         <v>33</v>
       </c>
       <c r="L32" s="4" t="s">
-        <v>53</v>
+        <v>35</v>
       </c>
       <c r="M32" s="32">
         <v>42089</v>
@@ -4281,7 +4306,7 @@
         <v>116</v>
       </c>
       <c r="O32" s="10" t="s">
-        <v>120</v>
+        <v>196</v>
       </c>
       <c r="P32" s="10"/>
     </row>
@@ -4290,7 +4315,7 @@
         <v>96</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="C33" s="3" t="s">
         <v>58</v>
@@ -4320,7 +4345,7 @@
         <v>33</v>
       </c>
       <c r="L33" s="4" t="s">
-        <v>53</v>
+        <v>35</v>
       </c>
       <c r="M33" s="32">
         <v>42089</v>
@@ -4329,7 +4354,7 @@
         <v>116</v>
       </c>
       <c r="O33" s="9" t="s">
-        <v>125</v>
+        <v>195</v>
       </c>
       <c r="P33" s="10"/>
     </row>
@@ -4338,7 +4363,7 @@
         <v>97</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="C34" s="3" t="s">
         <v>58</v>
@@ -5954,7 +5979,7 @@
           <x14:formula1>
             <xm:f>Settings!$F$4:$F$8</xm:f>
           </x14:formula1>
-          <xm:sqref>L2:L26 L30 L34</xm:sqref>
+          <xm:sqref>L34 L2:L26 L29</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
@@ -5990,8 +6015,8 @@
   </sheetPr>
   <dimension ref="A1:M34"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -6038,13 +6063,13 @@
         <v>66</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>61</v>
+        <v>199</v>
       </c>
       <c r="F2" s="1"/>
       <c r="H2" s="27" t="s">
@@ -6064,10 +6089,10 @@
         <v>67</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>61</v>
@@ -6089,10 +6114,10 @@
         <v>68</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>61</v>
@@ -6114,10 +6139,10 @@
         <v>69</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>61</v>
@@ -6139,10 +6164,10 @@
         <v>70</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>61</v>
@@ -6164,10 +6189,10 @@
         <v>71</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>61</v>
@@ -6189,10 +6214,10 @@
         <v>72</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>61</v>
@@ -6214,10 +6239,10 @@
         <v>73</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>61</v>
@@ -6239,10 +6264,10 @@
         <v>74</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>61</v>
@@ -6264,10 +6289,10 @@
         <v>115</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>61</v>
@@ -6289,10 +6314,10 @@
         <v>75</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>61</v>
@@ -6314,10 +6339,10 @@
         <v>76</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>61</v>
@@ -6339,10 +6364,10 @@
         <v>77</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>61</v>
@@ -6364,10 +6389,10 @@
         <v>78</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>61</v>
@@ -6389,10 +6414,10 @@
         <v>79</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>61</v>
@@ -6414,10 +6439,10 @@
         <v>80</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>61</v>
@@ -6439,10 +6464,10 @@
         <v>81</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>61</v>
@@ -6674,6 +6699,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C0A86D0A1DF85A4CBF24319CD50F658E" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="18023c554c1e7c0fe5f8bda126dbbbe1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c64490b4aec6201516c3a874156f37b2">
     <xsd:element name="properties">
@@ -6787,22 +6827,30 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A346E62E-1A2C-4E03-B91F-FE4FC47F8E89}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FEF49AB9-68C3-4E70-84F5-930D4AF0373D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{64745CD4-DB27-427B-80D9-1CCB91D6E4BC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6816,27 +6864,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A346E62E-1A2C-4E03-B91F-FE4FC47F8E89}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FEF49AB9-68C3-4E70-84F5-930D4AF0373D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
updates and changes for Jack
</commit_message>
<xml_diff>
--- a/Testing Spreadsheet v1.0 Order Page Meat Extravaganza pizza - Adam Hale.xlsx
+++ b/Testing Spreadsheet v1.0 Order Page Meat Extravaganza pizza - Adam Hale.xlsx
@@ -5,7 +5,7 @@
   <workbookPr autoCompressPictures="0"/>
   <workbookProtection workbookPassword="A6C2" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="24600" windowHeight="15360" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="24600" windowHeight="15360" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Reqs" sheetId="5" r:id="rId1"/>
@@ -200,7 +200,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="204">
   <si>
     <t xml:space="preserve">Req </t>
   </si>
@@ -842,6 +842,12 @@
   </si>
   <si>
     <t>The pizza is the wrong price due to incorrect pizza price. Failed on all browsers and mobile devices</t>
+  </si>
+  <si>
+    <t>Automated Selenium Test involving a manual intervention</t>
+  </si>
+  <si>
+    <t>Automated Selenium  Test involving a manual intervention</t>
   </si>
 </sst>
 </file>
@@ -2008,7 +2014,6 @@
           <c:dLbls>
             <c:dLbl>
               <c:idx val="0"/>
-              <c:layout/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
               <c:showCatName val="0"/>
@@ -2023,7 +2028,6 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="1"/>
-              <c:layout/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
               <c:showCatName val="0"/>
@@ -2109,7 +2113,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2200,11 +2203,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2120176824"/>
-        <c:axId val="2120179768"/>
+        <c:axId val="2122906568"/>
+        <c:axId val="2120953784"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2120176824"/>
+        <c:axId val="2122906568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2214,7 +2217,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2120179768"/>
+        <c:crossAx val="2120953784"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2222,7 +2225,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2120179768"/>
+        <c:axId val="2120953784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2233,7 +2236,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2120176824"/>
+        <c:crossAx val="2122906568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2814,7 +2817,7 @@
   </sheetPr>
   <dimension ref="A1:U146"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
+    <sheetView topLeftCell="A28" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
       <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
@@ -6042,8 +6045,8 @@
   </sheetPr>
   <dimension ref="A1:M34"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -6297,7 +6300,7 @@
         <v>143</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>61</v>
+        <v>202</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
@@ -6322,7 +6325,7 @@
         <v>144</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>61</v>
+        <v>202</v>
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
@@ -6347,7 +6350,7 @@
         <v>145</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>61</v>
+        <v>202</v>
       </c>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
@@ -6372,7 +6375,7 @@
         <v>146</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>61</v>
+        <v>202</v>
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
@@ -6397,7 +6400,7 @@
         <v>147</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>61</v>
+        <v>202</v>
       </c>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
@@ -6422,7 +6425,7 @@
         <v>148</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>61</v>
+        <v>202</v>
       </c>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
@@ -6447,7 +6450,7 @@
         <v>149</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>61</v>
+        <v>202</v>
       </c>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
@@ -6472,7 +6475,7 @@
         <v>150</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>61</v>
+        <v>202</v>
       </c>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
@@ -6497,7 +6500,7 @@
         <v>151</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>61</v>
+        <v>203</v>
       </c>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
@@ -6726,12 +6729,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C0A86D0A1DF85A4CBF24319CD50F658E" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="18023c554c1e7c0fe5f8bda126dbbbe1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c64490b4aec6201516c3a874156f37b2">
     <xsd:element name="properties">
@@ -6845,7 +6842,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -6854,22 +6851,13 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FEF49AB9-68C3-4E70-84F5-930D4AF0373D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{64745CD4-DB27-427B-80D9-1CCB91D6E4BC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6885,10 +6873,25 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A346E62E-1A2C-4E03-B91F-FE4FC47F8E89}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FEF49AB9-68C3-4E70-84F5-930D4AF0373D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
final tests for meat Ex pizza
</commit_message>
<xml_diff>
--- a/Testing Spreadsheet v1.0 Order Page Meat Extravaganza pizza - Adam Hale.xlsx
+++ b/Testing Spreadsheet v1.0 Order Page Meat Extravaganza pizza - Adam Hale.xlsx
@@ -5,7 +5,7 @@
   <workbookPr autoCompressPictures="0"/>
   <workbookProtection workbookPassword="A6C2" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="24600" windowHeight="15360" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24840" windowHeight="15600" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Reqs" sheetId="5" r:id="rId1"/>
@@ -200,7 +200,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="632" uniqueCount="234">
   <si>
     <t xml:space="preserve">Req </t>
   </si>
@@ -418,12 +418,6 @@
     <t>N/A</t>
   </si>
   <si>
-    <t>Tcase_10</t>
-  </si>
-  <si>
-    <t>Automated Selenium Test</t>
-  </si>
-  <si>
     <t>Order_TConn_1</t>
   </si>
   <si>
@@ -601,9 +595,6 @@
     <t>On adding the meat extravaganza pizza, with pepperoni to the basket.</t>
   </si>
   <si>
-    <t>On adding the meatextravaganza pizza, with peppers to the basket.</t>
-  </si>
-  <si>
     <t>On adding the meat extravaganza pizza, with onions to the basket.</t>
   </si>
   <si>
@@ -628,9 +619,6 @@
     <t>On adding the meat extravaganza pizza, with pepperoni, peppers and onions to the basket.</t>
   </si>
   <si>
-    <t>On adding the meat extravaganza pizza, with olives, peppers and onions to the basket.</t>
-  </si>
-  <si>
     <t>On adding the meat extravaganza pizza, with olives, pepperoni and onions to the basket.</t>
   </si>
   <si>
@@ -646,24 +634,9 @@
     <t>The meat extravaganza pizza is displayed in the basket. The correct price is displayed in the basket.</t>
   </si>
   <si>
-    <t>The meat extravaganza pizza with Olives is displayed in the basket. The correct price is displayed in the basket.</t>
-  </si>
-  <si>
     <t>The meat extravaganza pizza with pepperoni is displayed in the basket. The correct price is displayed in the basket.</t>
   </si>
   <si>
-    <t>The meat extravaganza pizza with peppers is displayed in the basket. The correct price is displayed in the basket.</t>
-  </si>
-  <si>
-    <t>The meat extravaganza pizza with onions is displayed in the basket. The correct price is displayed in the basket.</t>
-  </si>
-  <si>
-    <t>The meat extravaganza pizza with olives and pepperoni is displayed in the basket. The correct price is displayed in the basket.</t>
-  </si>
-  <si>
-    <t>The meatextravaganza pizza with olives and peppers is displayed in the basket. The correct price is displayed in the basket.</t>
-  </si>
-  <si>
     <t>The meat extravaganza pizza with olives and onions is displayed in the basket. The correct price is displayed in the basket.</t>
   </si>
   <si>
@@ -685,9 +658,6 @@
     <t>The meat extravaganza pizza with olives, pepperoni and onions is displayed in the basket. The correct price is displayed in the basket.</t>
   </si>
   <si>
-    <t>The meat extravaganza pizza with olives, pepperoni and peppers is displayed in the basket. The correct price is displayed in the basket.</t>
-  </si>
-  <si>
     <t>The meat extravaganza pizza with olives, pepperoni, peppers and onions is displayed in the basket. The correct price is displayed in the basket.</t>
   </si>
   <si>
@@ -757,36 +727,15 @@
     <t>Check that the correct price is displayed after the meat extravaganza pizza, with Peppers and Onions, is added to the cart</t>
   </si>
   <si>
-    <t>Check that I can select the meat extravaganza pizza, with Pepperoni, Peppers and Onions and add it to the cart.</t>
-  </si>
-  <si>
-    <t>Check that the correct price is displayed after the meat extravaganza pizza, with Pepperoni, Peppers and Onions, is added to the cart</t>
-  </si>
-  <si>
-    <t>Check that I can select the meat extravaganza pizza, with Olives, Peppers and Onions and add it too the cart.</t>
-  </si>
-  <si>
-    <t>Check that the correct price is displayed after the meat extravaganza pizza, with Olives, Peppers and Onions, is added to the cart</t>
-  </si>
-  <si>
     <t>Check that I can select the meat extravaganza pizza, with Olives, Pepperoni and Onions and add it too the cart.</t>
   </si>
   <si>
     <t>Check that the correct price is displayed after the meat extravaganza pizza, with Olives, Pepperoni and Onions, is added to the cart</t>
   </si>
   <si>
-    <t>Check that I can select the meat extravaganza pizza, with Olives, Pepperoni and Peppers and add it too the cart.</t>
-  </si>
-  <si>
-    <t>Check that the correct price is displayed after the meat extravaganza pizza, with Olives, Pepperoni and Peppers, is added to the cart</t>
-  </si>
-  <si>
     <t>Check that I can select the meat extravaganza pizza, with Olives, Pepperoni, Peppers and Onions and add it too the cart.</t>
   </si>
   <si>
-    <t>Check that the correct price is displayed after the meat extravaganza pizza, with Olives, Pepperoni, Peppers and Onions, is added to the cart</t>
-  </si>
-  <si>
     <t>Check that I can remove the meat extravaganza pizza with optional toppings from the basket.</t>
   </si>
   <si>
@@ -805,9 +754,6 @@
     <t>The onions topping was not added to cart. Failed on all browsers and mobile devices</t>
   </si>
   <si>
-    <t>total was incorrect due to incorrect pizza price as well as not adding onions to the cart. Failed on all browsers and mobile devices</t>
-  </si>
-  <si>
     <t>total was incorrect due to incorrect pizza price. Failed on all browsers and mobile devices</t>
   </si>
   <si>
@@ -826,15 +772,6 @@
     <t>The onions topping was not added to cart.  Failed on all browsers and mobile devices</t>
   </si>
   <si>
-    <t>total was incorrect due to incorrect pizza price as well as not adding onions to the cart.  Failed on all browsers and mobile devices</t>
-  </si>
-  <si>
-    <t>The total amount is incorrect due to both incorrect pizza price and extra price for peppers.  Failed on all browsers and mobile devices</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Automated Selenium Test </t>
-  </si>
-  <si>
     <t>Order_Tconn_3</t>
   </si>
   <si>
@@ -848,13 +785,166 @@
   </si>
   <si>
     <t>Automated Selenium  Test involving a manual intervention</t>
+  </si>
+  <si>
+    <t>The meat extravaganza pizza is displayed in the basket</t>
+  </si>
+  <si>
+    <t>The meat extravaganza pizza with olives is displayed in the basket. The correct price is displayed in the basket.</t>
+  </si>
+  <si>
+    <t>The meat extravaganza pizza with olives is displayed in the basket</t>
+  </si>
+  <si>
+    <t>The meat extravaganza pizza with pepperoni is displayed in the basket</t>
+  </si>
+  <si>
+    <t>On adding the meat extravaganza pizza, with  peppers to the basket.</t>
+  </si>
+  <si>
+    <t>The meatextravaganza pizza  peppers is displayed in the basket.</t>
+  </si>
+  <si>
+    <t>The meat extravaganza pizza with pepers is displayed in the basket. The correct price is displayed in the basket.</t>
+  </si>
+  <si>
+    <t>The meat extravaganza pizza with onions is displayed in the basket</t>
+  </si>
+  <si>
+    <t>The meat extravaganza pizza with onions is displayed in the basket. The correct price is displayed in the basket</t>
+  </si>
+  <si>
+    <t>The meat extravaganza pizza with olives and pepperonis is displayed in the basket</t>
+  </si>
+  <si>
+    <t>The meat extravaganza pizza with olives and pepperonis is displayed in the basket. The correct price is displayed in the basket.</t>
+  </si>
+  <si>
+    <t>The meat extravaganza pizza with olives and peppers is displayed in the basket</t>
+  </si>
+  <si>
+    <t>The meat extravaganza pizza with olives and peppers is displayed in the basket. The correct price is displayed in the basket.</t>
+  </si>
+  <si>
+    <t>The meat extravaganza pizza with olives and onions is displayed in the basket</t>
+  </si>
+  <si>
+    <t>The meat extravaganza pizza with pepperoni and peppers is displayed in the basket</t>
+  </si>
+  <si>
+    <t>On adding the meat extravaganza pizza, with pepperoni and onios to the basket.</t>
+  </si>
+  <si>
+    <t>The meat extravaganza pizza with pepperoni and onions is displayed in the basket</t>
+  </si>
+  <si>
+    <t>The meat extravaganza pizza with peppers and onions is displayed in the basket</t>
+  </si>
+  <si>
+    <t>Check that the correct price is displayed after the meat extravaganza pizza, with Olives, Pepperoni, Peppers and Onions, is added to the cart having the correct price</t>
+  </si>
+  <si>
+    <t>Order_TProc_18</t>
+  </si>
+  <si>
+    <t>Order_TProc_19</t>
+  </si>
+  <si>
+    <t>Order_TProc_20</t>
+  </si>
+  <si>
+    <t>Order_TProc_21</t>
+  </si>
+  <si>
+    <t>Order_TProc_22</t>
+  </si>
+  <si>
+    <t>Order_TProc_23</t>
+  </si>
+  <si>
+    <t>Order_TProc_24</t>
+  </si>
+  <si>
+    <t>Order_TProc_25</t>
+  </si>
+  <si>
+    <t>Order_TProc_26</t>
+  </si>
+  <si>
+    <t>Order_TProc_27</t>
+  </si>
+  <si>
+    <t>Order_TProc_28</t>
+  </si>
+  <si>
+    <t>Order_TProc_29</t>
+  </si>
+  <si>
+    <t>Order_TProc_30</t>
+  </si>
+  <si>
+    <t>Order_TProc_31</t>
+  </si>
+  <si>
+    <t>Order_TProc_32</t>
+  </si>
+  <si>
+    <t>Order_TProc_33</t>
+  </si>
+  <si>
+    <t>The meat extravaganza pizza with olives, pepperoni, peppers and olives to the basket</t>
+  </si>
+  <si>
+    <t>On adding the meat extravaganza pizza, with olives, peppers and onions to the basket</t>
+  </si>
+  <si>
+    <t>The meat extravaganza pizza with olives, peppers and onions is displayed in the basket</t>
+  </si>
+  <si>
+    <t>The meat extravaganza pizza with pepperoni, peppers and onions is displayed in the basket</t>
+  </si>
+  <si>
+    <t>The meat extravaganza pizza with olives, pepperoni and onions is displayed in the basket</t>
+  </si>
+  <si>
+    <t>The meat extravaganza pizza with olives, pepperoni and peppers s is displayed in the basket. The correct price is displayed in the basket.</t>
+  </si>
+  <si>
+    <t>The meat extravaganza pizza with olives, pepperoni and peppers is displayed in the basket</t>
+  </si>
+  <si>
+    <t>Check that I can select the meat extravaganza pizza, with olives, pepperoni and peppers and add it to the cart.</t>
+  </si>
+  <si>
+    <t>Check that the correct price is displayed after the meat extravaganza pizza, with olives, pepperoni and peppers  is added to the cart</t>
+  </si>
+  <si>
+    <t>Check that I can select the meat extravaganza pizza, with pepperoni, peppers and onions and add it too the cart.</t>
+  </si>
+  <si>
+    <t>Check that the correct price is displayed after the meat extravaganza pizza, with Olives, Pepperoni and onions, is added to the cart</t>
+  </si>
+  <si>
+    <t>The total amount is incorrect due to incorrect pizza price and onions not being added to cart and included in the price. Failed on all browsers and mobile devices</t>
+  </si>
+  <si>
+    <t>The total amount is incorrect due to both incorrect pizza price and extra price for peppers as well as the onions topping was not added to cart and not being included in the price.  Failed on all browsers and mobile devices</t>
+  </si>
+  <si>
+    <t>The total amount is incorrect due to both incorrect pizza price and extra price for peppers as well as the onions topping was not added to car and price being included.  Failed on all browsers and mobile devices</t>
+  </si>
+  <si>
+    <t>Check that the correct price is displayed after the e meat extravaganza pizza, with pepperoni, peppers and onions and add it too the cart.</t>
+  </si>
+  <si>
+    <t>Check that I can select the meat extravaganza pizza, with Olives, Pepperoni and onions, is added to the cart</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -968,6 +1058,23 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -1053,7 +1160,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="403">
+  <cellStyleXfs count="571">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1457,8 +1564,176 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1550,8 +1825,41 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="403">
+  <cellStyles count="571">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1753,6 +2061,90 @@
     <cellStyle name="Followed Hyperlink" xfId="398" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="400" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="402" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="404" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="406" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="408" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="410" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="412" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="414" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="416" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="418" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="420" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="422" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="424" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="426" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="428" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="430" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="432" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="434" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="436" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="438" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="440" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="442" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="444" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="446" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="448" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="450" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="452" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="454" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="456" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="458" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="460" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="462" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="464" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="466" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="468" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="470" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="472" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="474" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="476" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="478" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="480" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="482" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="484" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="486" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="488" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="490" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="492" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="494" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="496" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="498" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="500" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="502" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="504" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="506" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="508" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="510" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="512" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="514" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="516" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="518" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="520" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="522" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="524" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="526" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="528" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="530" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="532" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="534" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="536" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="538" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="540" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="542" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="544" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="546" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="548" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="550" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="552" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="554" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="556" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="558" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="560" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="562" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="564" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="566" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="568" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="570" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1954,6 +2346,90 @@
     <cellStyle name="Hyperlink" xfId="397" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="399" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="401" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="403" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="405" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="407" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="409" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="411" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="413" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="415" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="417" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="419" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="421" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="423" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="425" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="427" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="429" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="431" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="433" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="435" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="437" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="439" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="441" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="443" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="445" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="447" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="449" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="451" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="453" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="455" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="457" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="459" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="461" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="463" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="465" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="467" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="469" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="471" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="473" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="475" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="477" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="479" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="481" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="483" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="485" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="487" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="489" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="491" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="493" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="495" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="497" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="499" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="501" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="503" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="505" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="507" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="509" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="511" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="513" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="515" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="517" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="519" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="521" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="523" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="525" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="527" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="529" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="531" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="533" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="535" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="537" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="539" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="541" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="543" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="545" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="547" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="549" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="551" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="553" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="555" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="557" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="559" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="561" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="563" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="565" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="567" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="569" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="1">
@@ -2014,6 +2490,7 @@
           <c:dLbls>
             <c:dLbl>
               <c:idx val="0"/>
+              <c:layout/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
               <c:showCatName val="0"/>
@@ -2028,6 +2505,7 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="1"/>
+              <c:layout/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
               <c:showCatName val="0"/>
@@ -2113,6 +2591,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2203,11 +2682,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2122906568"/>
-        <c:axId val="2120953784"/>
+        <c:axId val="2066412984"/>
+        <c:axId val="2066415928"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2122906568"/>
+        <c:axId val="2066412984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2217,7 +2696,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2120953784"/>
+        <c:crossAx val="2066415928"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2225,7 +2704,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2120953784"/>
+        <c:axId val="2066415928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2236,7 +2715,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2122906568"/>
+        <c:crossAx val="2066412984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2676,10 +3155,10 @@
     </row>
     <row r="2" spans="1:9" ht="44" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>184</v>
+        <v>167</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>55</v>
@@ -2693,10 +3172,10 @@
     </row>
     <row r="3" spans="1:9" ht="69.5" customHeight="1">
       <c r="A3" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>185</v>
+        <v>168</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>55</v>
@@ -2708,7 +3187,7 @@
     </row>
     <row r="4" spans="1:9" ht="36.5" customHeight="1">
       <c r="A4" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>56</v>
@@ -2817,8 +3296,8 @@
   </sheetPr>
   <dimension ref="A1:U146"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="50" zoomScaleNormal="50" zoomScalePageLayoutView="50" workbookViewId="0">
+      <selection activeCell="O34" sqref="O34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -2890,10 +3369,10 @@
     </row>
     <row r="2" spans="1:21" ht="39">
       <c r="A2" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>58</v>
@@ -2902,7 +3381,7 @@
         <v>59</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F2" s="11" t="s">
         <v>6</v>
@@ -2914,7 +3393,7 @@
         <v>24</v>
       </c>
       <c r="I2" s="12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J2" s="3"/>
       <c r="K2" s="4"/>
@@ -2929,10 +3408,10 @@
     </row>
     <row r="3" spans="1:21" ht="52">
       <c r="A3" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>58</v>
@@ -2941,7 +3420,7 @@
         <v>59</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F3" s="11" t="s">
         <v>6</v>
@@ -2953,10 +3432,10 @@
         <v>25</v>
       </c>
       <c r="I3" s="12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="K3" s="4" t="s">
         <v>33</v>
@@ -2968,10 +3447,10 @@
         <v>42089</v>
       </c>
       <c r="N3" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="O3" s="9" t="s">
-        <v>201</v>
+        <v>180</v>
       </c>
       <c r="P3" s="10"/>
       <c r="T3" s="27" t="s">
@@ -2980,10 +3459,10 @@
     </row>
     <row r="4" spans="1:21" ht="52">
       <c r="A4" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>154</v>
+        <v>144</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>58</v>
@@ -2992,7 +3471,7 @@
         <v>59</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F4" s="11" t="s">
         <v>6</v>
@@ -3004,7 +3483,7 @@
         <v>24</v>
       </c>
       <c r="I4" s="12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J4" s="9"/>
       <c r="K4" s="4"/>
@@ -3016,10 +3495,10 @@
     </row>
     <row r="5" spans="1:21" ht="52">
       <c r="A5" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>58</v>
@@ -3028,7 +3507,7 @@
         <v>59</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F5" s="11" t="s">
         <v>6</v>
@@ -3040,10 +3519,10 @@
         <v>25</v>
       </c>
       <c r="I5" s="12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J5" s="9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="K5" s="4" t="s">
         <v>33</v>
@@ -3055,19 +3534,19 @@
         <v>42089</v>
       </c>
       <c r="N5" s="9" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="O5" s="9" t="s">
-        <v>186</v>
+        <v>169</v>
       </c>
       <c r="P5" s="10"/>
     </row>
     <row r="6" spans="1:21" ht="52">
-      <c r="A6" s="1" t="s">
-        <v>70</v>
+      <c r="A6" s="3" t="s">
+        <v>68</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>58</v>
@@ -3076,7 +3555,7 @@
         <v>59</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F6" s="11" t="s">
         <v>6</v>
@@ -3088,7 +3567,7 @@
         <v>24</v>
       </c>
       <c r="I6" s="12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J6" s="10"/>
       <c r="K6" s="4"/>
@@ -3106,11 +3585,11 @@
       </c>
     </row>
     <row r="7" spans="1:21" ht="65">
-      <c r="A7" s="1" t="s">
-        <v>71</v>
+      <c r="A7" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>58</v>
@@ -3119,7 +3598,7 @@
         <v>59</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F7" s="11" t="s">
         <v>6</v>
@@ -3131,10 +3610,10 @@
         <v>25</v>
       </c>
       <c r="I7" s="12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J7" s="10" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="K7" s="4" t="s">
         <v>33</v>
@@ -3146,10 +3625,10 @@
         <v>42089</v>
       </c>
       <c r="N7" s="10" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="O7" s="9" t="s">
-        <v>186</v>
+        <v>169</v>
       </c>
       <c r="P7" s="10"/>
       <c r="T7" t="s">
@@ -3162,10 +3641,10 @@
     </row>
     <row r="8" spans="1:21" ht="52">
       <c r="A8" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>58</v>
@@ -3174,7 +3653,7 @@
         <v>59</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F8" s="11" t="s">
         <v>6</v>
@@ -3186,7 +3665,7 @@
         <v>24</v>
       </c>
       <c r="I8" s="12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J8" s="10"/>
       <c r="K8" s="4"/>
@@ -3198,10 +3677,10 @@
     </row>
     <row r="9" spans="1:21" ht="52">
       <c r="A9" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>58</v>
@@ -3210,7 +3689,7 @@
         <v>59</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F9" s="11" t="s">
         <v>6</v>
@@ -3222,10 +3701,10 @@
         <v>25</v>
       </c>
       <c r="I9" s="12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J9" s="10" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="K9" s="4" t="s">
         <v>33</v>
@@ -3237,19 +3716,19 @@
         <v>42089</v>
       </c>
       <c r="N9" s="10" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="O9" s="9" t="s">
-        <v>187</v>
+        <v>170</v>
       </c>
       <c r="P9" s="10"/>
     </row>
     <row r="10" spans="1:21" ht="52">
       <c r="A10" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>58</v>
@@ -3258,7 +3737,7 @@
         <v>59</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F10" s="11" t="s">
         <v>6</v>
@@ -3270,10 +3749,10 @@
         <v>25</v>
       </c>
       <c r="I10" s="12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J10" s="10" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="K10" s="4" t="s">
         <v>33</v>
@@ -3285,19 +3764,19 @@
         <v>42089</v>
       </c>
       <c r="N10" s="10" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="O10" s="10" t="s">
-        <v>188</v>
+        <v>171</v>
       </c>
       <c r="P10" s="10"/>
     </row>
     <row r="11" spans="1:21" ht="52">
       <c r="A11" s="3" t="s">
-        <v>60</v>
+        <v>113</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>58</v>
@@ -3306,7 +3785,7 @@
         <v>59</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F11" s="11" t="s">
         <v>6</v>
@@ -3318,10 +3797,10 @@
         <v>25</v>
       </c>
       <c r="I11" s="12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J11" s="10" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="K11" s="4" t="s">
         <v>33</v>
@@ -3333,19 +3812,19 @@
         <v>42089</v>
       </c>
       <c r="N11" s="10" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="O11" s="10" t="s">
-        <v>189</v>
+        <v>229</v>
       </c>
       <c r="P11" s="10"/>
     </row>
     <row r="12" spans="1:21" ht="52">
       <c r="A12" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>161</v>
+        <v>151</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>58</v>
@@ -3354,7 +3833,7 @@
         <v>59</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F12" s="11" t="s">
         <v>6</v>
@@ -3366,7 +3845,7 @@
         <v>24</v>
       </c>
       <c r="I12" s="12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J12" s="10"/>
       <c r="K12" s="10"/>
@@ -3378,10 +3857,10 @@
     </row>
     <row r="13" spans="1:21" ht="65">
       <c r="A13" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>58</v>
@@ -3390,7 +3869,7 @@
         <v>59</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F13" s="11" t="s">
         <v>6</v>
@@ -3402,10 +3881,10 @@
         <v>25</v>
       </c>
       <c r="I13" s="12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J13" s="10" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="K13" s="4" t="s">
         <v>33</v>
@@ -3417,19 +3896,19 @@
         <v>42089</v>
       </c>
       <c r="N13" s="10" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="O13" s="10" t="s">
-        <v>190</v>
+        <v>172</v>
       </c>
       <c r="P13" s="10"/>
     </row>
     <row r="14" spans="1:21" ht="52">
       <c r="A14" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>58</v>
@@ -3438,7 +3917,7 @@
         <v>59</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F14" s="11" t="s">
         <v>6</v>
@@ -3450,7 +3929,7 @@
         <v>24</v>
       </c>
       <c r="I14" s="12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J14" s="10"/>
       <c r="K14" s="10"/>
@@ -3462,10 +3941,10 @@
     </row>
     <row r="15" spans="1:21" ht="65">
       <c r="A15" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>58</v>
@@ -3474,7 +3953,7 @@
         <v>59</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F15" s="11" t="s">
         <v>6</v>
@@ -3486,10 +3965,10 @@
         <v>25</v>
       </c>
       <c r="I15" s="12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J15" s="10" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="K15" s="4" t="s">
         <v>33</v>
@@ -3501,19 +3980,19 @@
         <v>42089</v>
       </c>
       <c r="N15" s="10" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="O15" s="9" t="s">
-        <v>191</v>
+        <v>173</v>
       </c>
       <c r="P15" s="10"/>
     </row>
     <row r="16" spans="1:21" ht="52">
       <c r="A16" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>58</v>
@@ -3522,7 +4001,7 @@
         <v>59</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F16" s="11" t="s">
         <v>6</v>
@@ -3534,10 +4013,10 @@
         <v>25</v>
       </c>
       <c r="I16" s="12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J16" s="10" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="K16" s="4" t="s">
         <v>33</v>
@@ -3549,19 +4028,19 @@
         <v>42089</v>
       </c>
       <c r="N16" s="10" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="O16" s="10" t="s">
-        <v>188</v>
+        <v>171</v>
       </c>
       <c r="P16" s="10"/>
     </row>
     <row r="17" spans="1:21" ht="65">
       <c r="A17" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>58</v>
@@ -3570,7 +4049,7 @@
         <v>59</v>
       </c>
       <c r="E17" s="11" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F17" s="11" t="s">
         <v>6</v>
@@ -3582,10 +4061,10 @@
         <v>25</v>
       </c>
       <c r="I17" s="12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J17" s="10" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="K17" s="4" t="s">
         <v>33</v>
@@ -3597,19 +4076,19 @@
         <v>42089</v>
       </c>
       <c r="N17" s="10" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="O17" s="10" t="s">
-        <v>189</v>
+        <v>229</v>
       </c>
       <c r="P17" s="10"/>
     </row>
     <row r="18" spans="1:21" ht="52">
       <c r="A18" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>58</v>
@@ -3618,7 +4097,7 @@
         <v>59</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F18" s="11" t="s">
         <v>6</v>
@@ -3630,7 +4109,7 @@
         <v>24</v>
       </c>
       <c r="I18" s="12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J18" s="10"/>
       <c r="K18" s="10"/>
@@ -3649,10 +4128,10 @@
     </row>
     <row r="19" spans="1:21" ht="65">
       <c r="A19" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>58</v>
@@ -3673,10 +4152,10 @@
         <v>25</v>
       </c>
       <c r="I19" s="12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J19" s="10" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="K19" s="4" t="s">
         <v>33</v>
@@ -3688,10 +4167,10 @@
         <v>42089</v>
       </c>
       <c r="N19" s="10" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="O19" s="9" t="s">
-        <v>192</v>
+        <v>174</v>
       </c>
       <c r="P19" s="10"/>
       <c r="T19" t="s">
@@ -3704,10 +4183,10 @@
     </row>
     <row r="20" spans="1:21" ht="52">
       <c r="A20" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>58</v>
@@ -3728,10 +4207,10 @@
         <v>25</v>
       </c>
       <c r="I20" s="12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J20" s="10" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="K20" s="4" t="s">
         <v>33</v>
@@ -3743,10 +4222,10 @@
         <v>42089</v>
       </c>
       <c r="N20" s="10" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="O20" s="10" t="s">
-        <v>193</v>
+        <v>175</v>
       </c>
       <c r="P20" s="10"/>
       <c r="T20" t="s">
@@ -3759,10 +4238,10 @@
     </row>
     <row r="21" spans="1:21" ht="65">
       <c r="A21" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>58</v>
@@ -3783,10 +4262,10 @@
         <v>25</v>
       </c>
       <c r="I21" s="12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J21" s="10" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="K21" s="4" t="s">
         <v>33</v>
@@ -3798,10 +4277,10 @@
         <v>42089</v>
       </c>
       <c r="N21" s="10" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="O21" s="10" t="s">
-        <v>189</v>
+        <v>229</v>
       </c>
       <c r="P21" s="10"/>
       <c r="T21" t="s">
@@ -3814,10 +4293,10 @@
     </row>
     <row r="22" spans="1:21" ht="52">
       <c r="A22" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>58</v>
@@ -3838,10 +4317,10 @@
         <v>25</v>
       </c>
       <c r="I22" s="12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J22" s="10" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="K22" s="4" t="s">
         <v>33</v>
@@ -3853,19 +4332,19 @@
         <v>42089</v>
       </c>
       <c r="N22" s="10" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="O22" s="10" t="s">
-        <v>188</v>
+        <v>171</v>
       </c>
       <c r="P22" s="10"/>
     </row>
     <row r="23" spans="1:21" ht="65">
       <c r="A23" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>58</v>
@@ -3886,10 +4365,10 @@
         <v>25</v>
       </c>
       <c r="I23" s="12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J23" s="10" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="K23" s="4" t="s">
         <v>33</v>
@@ -3901,19 +4380,19 @@
         <v>42089</v>
       </c>
       <c r="N23" s="10" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="O23" s="9" t="s">
-        <v>194</v>
+        <v>176</v>
       </c>
       <c r="P23" s="10"/>
     </row>
-    <row r="24" spans="1:21" ht="52">
+    <row r="24" spans="1:21" ht="65">
       <c r="A24" s="3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>173</v>
+        <v>225</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>58</v>
@@ -3931,37 +4410,35 @@
         <v>42089</v>
       </c>
       <c r="H24" s="26" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I24" s="12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J24" s="10" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="K24" s="4" t="s">
         <v>33</v>
       </c>
       <c r="L24" s="4" t="s">
-        <v>53</v>
+        <v>35</v>
       </c>
       <c r="M24" s="32">
         <v>42089</v>
       </c>
       <c r="N24" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="O24" s="10" t="s">
-        <v>195</v>
-      </c>
+        <v>114</v>
+      </c>
+      <c r="O24" s="10"/>
       <c r="P24" s="10"/>
     </row>
     <row r="25" spans="1:21" ht="65">
       <c r="A25" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>174</v>
+        <v>226</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>58</v>
@@ -3982,34 +4459,34 @@
         <v>25</v>
       </c>
       <c r="I25" s="12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J25" s="10" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="K25" s="4" t="s">
         <v>33</v>
       </c>
       <c r="L25" s="4" t="s">
-        <v>53</v>
+        <v>35</v>
       </c>
       <c r="M25" s="32">
         <v>42089</v>
       </c>
       <c r="N25" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="O25" s="9" t="s">
-        <v>194</v>
+        <v>114</v>
+      </c>
+      <c r="O25" s="45" t="s">
+        <v>170</v>
       </c>
       <c r="P25" s="10"/>
     </row>
     <row r="26" spans="1:21" ht="65">
       <c r="A26" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>175</v>
+        <v>87</v>
+      </c>
+      <c r="B26" s="44" t="s">
+        <v>163</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>58</v>
@@ -4030,34 +4507,34 @@
         <v>25</v>
       </c>
       <c r="I26" s="12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J26" s="10" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="K26" s="4" t="s">
         <v>33</v>
       </c>
       <c r="L26" s="4" t="s">
-        <v>53</v>
+        <v>35</v>
       </c>
       <c r="M26" s="32">
         <v>42089</v>
       </c>
       <c r="N26" s="10" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="O26" s="10" t="s">
-        <v>195</v>
+        <v>177</v>
       </c>
       <c r="P26" s="10"/>
     </row>
     <row r="27" spans="1:21" ht="65">
       <c r="A27" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>176</v>
+        <v>88</v>
+      </c>
+      <c r="B27" s="44" t="s">
+        <v>164</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>58</v>
@@ -4078,34 +4555,34 @@
         <v>25</v>
       </c>
       <c r="I27" s="12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J27" s="10" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="K27" s="4" t="s">
         <v>33</v>
       </c>
       <c r="L27" s="4" t="s">
-        <v>53</v>
+        <v>35</v>
       </c>
       <c r="M27" s="32">
         <v>42089</v>
       </c>
       <c r="N27" s="10" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="O27" s="9" t="s">
-        <v>194</v>
+        <v>231</v>
       </c>
       <c r="P27" s="10"/>
     </row>
     <row r="28" spans="1:21" ht="65">
       <c r="A28" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>177</v>
+        <v>89</v>
+      </c>
+      <c r="B28" s="44" t="s">
+        <v>227</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>58</v>
@@ -4126,58 +4603,58 @@
         <v>25</v>
       </c>
       <c r="I28" s="12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J28" s="10" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="K28" s="4" t="s">
         <v>33</v>
       </c>
       <c r="L28" s="4" t="s">
-        <v>53</v>
+        <v>35</v>
       </c>
       <c r="M28" s="32">
         <v>42089</v>
       </c>
       <c r="N28" s="10" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="O28" s="10" t="s">
-        <v>195</v>
+        <v>177</v>
       </c>
       <c r="P28" s="10"/>
     </row>
-    <row r="29" spans="1:21" ht="65">
+    <row r="29" spans="1:21" ht="78">
       <c r="A29" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>178</v>
-      </c>
-      <c r="C29" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B29" s="44" t="s">
+        <v>232</v>
+      </c>
+      <c r="C29" s="36" t="s">
         <v>58</v>
       </c>
-      <c r="D29" s="3" t="s">
+      <c r="D29" s="36" t="s">
         <v>59</v>
       </c>
-      <c r="E29" s="11" t="s">
+      <c r="E29" s="37" t="s">
         <v>54</v>
       </c>
-      <c r="F29" s="11" t="s">
+      <c r="F29" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="G29" s="13">
+      <c r="G29" s="38">
         <v>42089</v>
       </c>
-      <c r="H29" s="26" t="s">
+      <c r="H29" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="I29" s="12" t="s">
-        <v>65</v>
+      <c r="I29" s="40" t="s">
+        <v>63</v>
       </c>
       <c r="J29" s="10" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="K29" s="4" t="s">
         <v>33</v>
@@ -4189,79 +4666,91 @@
         <v>42089</v>
       </c>
       <c r="N29" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="O29" s="10" t="s">
-        <v>196</v>
+        <v>114</v>
+      </c>
+      <c r="O29" s="41" t="s">
+        <v>230</v>
       </c>
       <c r="P29" s="10"/>
     </row>
-    <row r="30" spans="1:21" ht="65">
+    <row r="30" spans="1:21" ht="52">
       <c r="A30" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="C30" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B30" s="44" t="s">
+        <v>233</v>
+      </c>
+      <c r="C30" s="36" t="s">
         <v>58</v>
       </c>
-      <c r="D30" s="3" t="s">
+      <c r="D30" s="36" t="s">
         <v>59</v>
       </c>
-      <c r="E30" s="11" t="s">
+      <c r="E30" s="37" t="s">
         <v>54</v>
       </c>
-      <c r="F30" s="11" t="s">
+      <c r="F30" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="G30" s="13">
+      <c r="G30" s="38">
         <v>42089</v>
       </c>
-      <c r="H30" s="26" t="s">
-        <v>24</v>
-      </c>
-      <c r="I30" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="J30" s="10"/>
-      <c r="K30" s="10"/>
-      <c r="L30" s="4"/>
-      <c r="M30" s="10"/>
-      <c r="N30" s="10"/>
-      <c r="O30" s="10"/>
+      <c r="H30" s="39" t="s">
+        <v>25</v>
+      </c>
+      <c r="I30" s="40" t="s">
+        <v>63</v>
+      </c>
+      <c r="J30" s="41" t="s">
+        <v>61</v>
+      </c>
+      <c r="K30" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="L30" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="M30" s="42">
+        <v>42089</v>
+      </c>
+      <c r="N30" s="41" t="s">
+        <v>114</v>
+      </c>
+      <c r="O30" s="43" t="s">
+        <v>177</v>
+      </c>
       <c r="P30" s="10"/>
     </row>
     <row r="31" spans="1:21" ht="65">
       <c r="A31" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="C31" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B31" s="44" t="s">
+        <v>228</v>
+      </c>
+      <c r="C31" s="36" t="s">
         <v>58</v>
       </c>
-      <c r="D31" s="3" t="s">
+      <c r="D31" s="36" t="s">
         <v>59</v>
       </c>
-      <c r="E31" s="11" t="s">
+      <c r="E31" s="37" t="s">
         <v>54</v>
       </c>
-      <c r="F31" s="11" t="s">
+      <c r="F31" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="G31" s="13">
+      <c r="G31" s="38">
         <v>42089</v>
       </c>
-      <c r="H31" s="26" t="s">
+      <c r="H31" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="I31" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="J31" s="10" t="s">
+      <c r="I31" s="40" t="s">
         <v>63</v>
+      </c>
+      <c r="J31" s="41" t="s">
+        <v>61</v>
       </c>
       <c r="K31" s="4" t="s">
         <v>33</v>
@@ -4269,47 +4758,47 @@
       <c r="L31" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="M31" s="32">
+      <c r="M31" s="42">
         <v>42089</v>
       </c>
-      <c r="N31" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="O31" s="9" t="s">
-        <v>197</v>
+      <c r="N31" s="41" t="s">
+        <v>114</v>
+      </c>
+      <c r="O31" s="41" t="s">
+        <v>229</v>
       </c>
       <c r="P31" s="10"/>
     </row>
     <row r="32" spans="1:21" ht="65">
       <c r="A32" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="C32" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B32" s="44" t="s">
+        <v>165</v>
+      </c>
+      <c r="C32" s="36" t="s">
         <v>58</v>
       </c>
-      <c r="D32" s="3" t="s">
+      <c r="D32" s="36" t="s">
         <v>59</v>
       </c>
-      <c r="E32" s="11" t="s">
+      <c r="E32" s="37" t="s">
         <v>54</v>
       </c>
-      <c r="F32" s="11" t="s">
+      <c r="F32" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="G32" s="13">
+      <c r="G32" s="38">
         <v>42089</v>
       </c>
-      <c r="H32" s="26" t="s">
+      <c r="H32" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="I32" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="J32" s="10" t="s">
+      <c r="I32" s="40" t="s">
         <v>63</v>
+      </c>
+      <c r="J32" s="41" t="s">
+        <v>61</v>
       </c>
       <c r="K32" s="4" t="s">
         <v>33</v>
@@ -4317,95 +4806,95 @@
       <c r="L32" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="M32" s="32">
+      <c r="M32" s="42">
         <v>42089</v>
       </c>
-      <c r="N32" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="O32" s="10" t="s">
-        <v>195</v>
+      <c r="N32" s="41" t="s">
+        <v>114</v>
+      </c>
+      <c r="O32" s="41" t="s">
+        <v>177</v>
       </c>
       <c r="P32" s="10"/>
     </row>
     <row r="33" spans="1:16" ht="78">
       <c r="A33" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="C33" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B33" s="44" t="s">
+        <v>201</v>
+      </c>
+      <c r="C33" s="36" t="s">
         <v>58</v>
       </c>
-      <c r="D33" s="3" t="s">
+      <c r="D33" s="36" t="s">
         <v>59</v>
       </c>
-      <c r="E33" s="11" t="s">
+      <c r="E33" s="37" t="s">
         <v>54</v>
       </c>
-      <c r="F33" s="11" t="s">
+      <c r="F33" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="G33" s="13">
+      <c r="G33" s="38">
         <v>42089</v>
       </c>
-      <c r="H33" s="26" t="s">
+      <c r="H33" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="I33" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="J33" s="10" t="s">
+      <c r="I33" s="40" t="s">
         <v>63</v>
       </c>
-      <c r="K33" s="4" t="s">
+      <c r="J33" s="41" t="s">
+        <v>61</v>
+      </c>
+      <c r="K33" s="34" t="s">
         <v>33</v>
       </c>
       <c r="L33" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="M33" s="32">
+      <c r="M33" s="42">
         <v>42089</v>
       </c>
-      <c r="N33" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="O33" s="9" t="s">
-        <v>194</v>
+      <c r="N33" s="41" t="s">
+        <v>114</v>
+      </c>
+      <c r="O33" s="41" t="s">
+        <v>230</v>
       </c>
       <c r="P33" s="10"/>
     </row>
     <row r="34" spans="1:16" ht="52">
       <c r="A34" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="C34" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B34" s="44" t="s">
+        <v>166</v>
+      </c>
+      <c r="C34" s="36" t="s">
         <v>58</v>
       </c>
-      <c r="D34" s="3" t="s">
+      <c r="D34" s="36" t="s">
         <v>59</v>
       </c>
-      <c r="E34" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="F34" s="11" t="s">
+      <c r="E34" s="37" t="s">
+        <v>62</v>
+      </c>
+      <c r="F34" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="G34" s="13">
+      <c r="G34" s="38">
         <v>42089</v>
       </c>
-      <c r="H34" s="26" t="s">
+      <c r="H34" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="I34" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="J34" s="10" t="s">
-        <v>199</v>
+      <c r="I34" s="40" t="s">
+        <v>63</v>
+      </c>
+      <c r="J34" s="41" t="s">
+        <v>178</v>
       </c>
       <c r="K34" s="34" t="s">
         <v>33</v>
@@ -4413,29 +4902,33 @@
       <c r="L34" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="M34" s="32">
+      <c r="M34" s="42">
         <v>42089</v>
       </c>
-      <c r="N34" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="O34" s="1" t="s">
-        <v>200</v>
+      <c r="N34" s="41" t="s">
+        <v>114</v>
+      </c>
+      <c r="O34" s="35" t="s">
+        <v>179</v>
       </c>
       <c r="P34" s="10"/>
     </row>
     <row r="35" spans="1:16">
-      <c r="E35" s="10"/>
+      <c r="A35" s="3"/>
+      <c r="B35" s="3"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="11"/>
       <c r="F35" s="11"/>
-      <c r="G35" s="10"/>
+      <c r="G35" s="13"/>
       <c r="H35" s="26"/>
       <c r="I35" s="12"/>
       <c r="J35" s="10"/>
-      <c r="K35" s="10"/>
-      <c r="L35" s="10"/>
-      <c r="M35" s="10"/>
+      <c r="K35" s="34"/>
+      <c r="L35" s="4"/>
+      <c r="M35" s="32"/>
       <c r="N35" s="10"/>
-      <c r="O35" s="10"/>
+      <c r="O35" s="1"/>
       <c r="P35" s="10"/>
     </row>
     <row r="36" spans="1:16">
@@ -5993,9 +6486,9 @@
       <c r="P146" s="10"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="H35:H144">
+  <conditionalFormatting sqref="H36:H144">
     <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="Passed ">
-      <formula>NOT(ISERROR(SEARCH("Passed ",H35)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Passed ",H36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6009,25 +6502,25 @@
           <x14:formula1>
             <xm:f>Settings!$F$4:$F$8</xm:f>
           </x14:formula1>
-          <xm:sqref>L34 L2:L26 L29</xm:sqref>
+          <xm:sqref>L35 L2:L23</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Settings!$D$4:$D$6</xm:f>
           </x14:formula1>
-          <xm:sqref>K2:K11 K13 K15:K17 K19:K29 K31:K33</xm:sqref>
+          <xm:sqref>K2:K11 K13 K15:K17 K19:K29</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Settings!$A$4:$A$6</xm:f>
           </x14:formula1>
-          <xm:sqref>H2:H34</xm:sqref>
+          <xm:sqref>H2:H28 H35</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Settings!$B$4:$B$6</xm:f>
           </x14:formula1>
-          <xm:sqref>F2:F144</xm:sqref>
+          <xm:sqref>F2:F28 F35:F144</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -6043,10 +6536,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor rgb="FF99FF99"/>
   </sheetPr>
-  <dimension ref="A1:M34"/>
+  <dimension ref="A1:M35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView topLeftCell="A23" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -6085,21 +6578,21 @@
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
     </row>
-    <row r="2" spans="1:13" ht="56">
+    <row r="2" spans="1:13" ht="42">
       <c r="A2" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>135</v>
+        <v>183</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>198</v>
+        <v>181</v>
       </c>
       <c r="F2" s="1"/>
       <c r="H2" s="27" t="s">
@@ -6113,19 +6606,19 @@
     </row>
     <row r="3" spans="1:13" ht="56">
       <c r="A3" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>61</v>
+        <v>181</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="1"/>
@@ -6136,21 +6629,21 @@
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
-    <row r="4" spans="1:13" ht="56">
+    <row r="4" spans="1:13" ht="42">
       <c r="A4" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>137</v>
+        <v>185</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>61</v>
+        <v>181</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
@@ -6163,19 +6656,19 @@
     </row>
     <row r="5" spans="1:13" ht="56">
       <c r="A5" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>138</v>
+        <v>184</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>61</v>
+        <v>181</v>
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
@@ -6186,21 +6679,21 @@
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
     </row>
-    <row r="6" spans="1:13" ht="56">
+    <row r="6" spans="1:13" ht="42">
       <c r="A6" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>139</v>
+        <v>186</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>61</v>
+        <v>181</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
@@ -6211,21 +6704,21 @@
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
     </row>
-    <row r="7" spans="1:13" ht="70">
+    <row r="7" spans="1:13" ht="56">
       <c r="A7" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>61</v>
+        <v>181</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
@@ -6236,21 +6729,21 @@
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
     </row>
-    <row r="8" spans="1:13" ht="70">
+    <row r="8" spans="1:13" ht="42">
       <c r="A8" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>124</v>
+        <v>187</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>141</v>
+        <v>188</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>61</v>
+        <v>181</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
@@ -6261,21 +6754,21 @@
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
     </row>
-    <row r="9" spans="1:13" ht="70">
+    <row r="9" spans="1:13" ht="56">
       <c r="A9" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>125</v>
+        <v>187</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>142</v>
+        <v>189</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>61</v>
+        <v>181</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
@@ -6286,21 +6779,21 @@
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
     </row>
-    <row r="10" spans="1:13" ht="70">
+    <row r="10" spans="1:13" ht="42">
       <c r="A10" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>143</v>
+        <v>190</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>202</v>
+        <v>181</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
@@ -6311,21 +6804,21 @@
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
     </row>
-    <row r="11" spans="1:13" ht="70">
+    <row r="11" spans="1:13" ht="56">
       <c r="A11" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>144</v>
+        <v>191</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>202</v>
+        <v>181</v>
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
@@ -6336,21 +6829,21 @@
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
     </row>
-    <row r="12" spans="1:13" ht="70">
+    <row r="12" spans="1:13" ht="42">
       <c r="A12" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>145</v>
+        <v>192</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>202</v>
+        <v>181</v>
       </c>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
@@ -6363,19 +6856,19 @@
     </row>
     <row r="13" spans="1:13" ht="70">
       <c r="A13" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>146</v>
+        <v>193</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>202</v>
+        <v>181</v>
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
@@ -6386,21 +6879,21 @@
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
     </row>
-    <row r="14" spans="1:13" ht="70">
+    <row r="14" spans="1:13" ht="42">
       <c r="A14" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>147</v>
+        <v>194</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>202</v>
+        <v>181</v>
       </c>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
@@ -6413,19 +6906,19 @@
     </row>
     <row r="15" spans="1:13" ht="70">
       <c r="A15" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>148</v>
+        <v>195</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>202</v>
+        <v>181</v>
       </c>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
@@ -6436,21 +6929,21 @@
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
     </row>
-    <row r="16" spans="1:13" ht="70">
+    <row r="16" spans="1:13" ht="42">
       <c r="A16" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>149</v>
+        <v>196</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>202</v>
+        <v>181</v>
       </c>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
@@ -6461,21 +6954,21 @@
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
     </row>
-    <row r="17" spans="1:13" ht="84">
+    <row r="17" spans="1:13" ht="70">
       <c r="A17" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C17" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="D17" s="1" t="s">
-        <v>150</v>
-      </c>
       <c r="E17" s="1" t="s">
-        <v>202</v>
+        <v>181</v>
       </c>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
@@ -6488,19 +6981,19 @@
     </row>
     <row r="18" spans="1:13" ht="42">
       <c r="A18" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>151</v>
+        <v>197</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>203</v>
+        <v>182</v>
       </c>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
@@ -6511,7 +7004,22 @@
       <c r="L18" s="1"/>
       <c r="M18" s="1"/>
     </row>
-    <row r="19" spans="1:13">
+    <row r="19" spans="1:13" ht="70">
+      <c r="A19" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>182</v>
+      </c>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
@@ -6521,110 +7029,267 @@
       <c r="L19" s="1"/>
       <c r="M19" s="1"/>
     </row>
-    <row r="20" spans="1:13">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-    </row>
-    <row r="21" spans="1:13">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-    </row>
-    <row r="22" spans="1:13">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-    </row>
-    <row r="23" spans="1:13">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-    </row>
-    <row r="24" spans="1:13">
-      <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-    </row>
-    <row r="25" spans="1:13">
-      <c r="A25" s="1"/>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-    </row>
-    <row r="26" spans="1:13">
-      <c r="A26" s="1"/>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-    </row>
-    <row r="27" spans="1:13">
-      <c r="A27" s="1"/>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-    </row>
-    <row r="28" spans="1:13">
-      <c r="A28" s="1"/>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-    </row>
-    <row r="29" spans="1:13">
-      <c r="A29" s="1"/>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-    </row>
-    <row r="30" spans="1:13">
-      <c r="A30" s="1"/>
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-    </row>
-    <row r="31" spans="1:13">
-      <c r="A31" s="1"/>
-      <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
-    </row>
-    <row r="32" spans="1:13">
-      <c r="A32" s="1"/>
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
-    </row>
-    <row r="33" spans="1:5">
-      <c r="A33" s="1"/>
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="1"/>
-      <c r="E33" s="1"/>
-    </row>
-    <row r="34" spans="1:5">
-      <c r="A34" s="1"/>
-      <c r="B34" s="1"/>
-      <c r="C34" s="1"/>
-      <c r="D34" s="1"/>
-      <c r="E34" s="1"/>
+    <row r="20" spans="1:13" ht="42">
+      <c r="A20" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="70">
+      <c r="A21" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" ht="42">
+      <c r="A22" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" ht="70">
+      <c r="A23" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" ht="56">
+      <c r="A24" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" ht="70">
+      <c r="A25" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" ht="56">
+      <c r="A26" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" ht="70">
+      <c r="A27" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" ht="56">
+      <c r="A28" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" ht="70">
+      <c r="A29" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" ht="56">
+      <c r="A30" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C30" s="35" t="s">
+        <v>219</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" ht="70">
+      <c r="A31" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C31" s="35" t="s">
+        <v>219</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" ht="56">
+      <c r="A32" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C32" s="35" t="s">
+        <v>129</v>
+      </c>
+      <c r="D32" s="35" t="s">
+        <v>218</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="84">
+      <c r="A33" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C33" s="35" t="s">
+        <v>129</v>
+      </c>
+      <c r="D33" s="35" t="s">
+        <v>140</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="42">
+      <c r="A34" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C34" s="35" t="s">
+        <v>130</v>
+      </c>
+      <c r="D34" s="35" t="s">
+        <v>141</v>
+      </c>
+      <c r="E34" s="35" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" s="1"/>
+      <c r="B35" s="1"/>
+      <c r="C35" s="35"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6729,6 +7394,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C0A86D0A1DF85A4CBF24319CD50F658E" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="18023c554c1e7c0fe5f8bda126dbbbe1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c64490b4aec6201516c3a874156f37b2">
     <xsd:element name="properties">
@@ -6842,22 +7522,30 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A346E62E-1A2C-4E03-B91F-FE4FC47F8E89}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FEF49AB9-68C3-4E70-84F5-930D4AF0373D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{64745CD4-DB27-427B-80D9-1CCB91D6E4BC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6871,27 +7559,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A346E62E-1A2C-4E03-B91F-FE4FC47F8E89}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FEF49AB9-68C3-4E70-84F5-930D4AF0373D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>